<commit_message>
Rewrote main to be a C++ file. Deleted HMI contents as they were no longer required. Also modified other files to work with C++
</commit_message>
<xml_diff>
--- a/doc/Project Management/Project Log Template.xlsx
+++ b/doc/Project Management/Project Log Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\great\Documents\GitHub\SD1_ndoherty\sd1_ndoherty\doc\Project Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\great\Documents\GitHub\SD1_ndoherty\doc\Project Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="290">
   <si>
     <t>Date:</t>
   </si>
@@ -769,12 +769,6 @@
   </si>
   <si>
     <t>Developer 1 Name:</t>
-  </si>
-  <si>
-    <t>Developer 2 Name:</t>
-  </si>
-  <si>
-    <t>Developer 3 Name:</t>
   </si>
   <si>
     <t>Developer 1:</t>
@@ -1520,6 +1514,24 @@
   </si>
   <si>
     <t>LOC Check Function</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>Coding the greeting and passing of variables</t>
+  </si>
+  <si>
+    <t>File Selection Function</t>
+  </si>
+  <si>
+    <t>LOC Counter Function</t>
+  </si>
+  <si>
+    <t>HMI Module</t>
+  </si>
+  <si>
+    <t>Coding an improved HMI Module</t>
   </si>
 </sst>
 </file>
@@ -2345,12 +2357,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2782,7 +2794,7 @@
   <dimension ref="B1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2798,15 +2810,15 @@
   <sheetData>
     <row r="1" spans="2:7" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B1" s="98" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B3" s="100" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D3" s="101" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="22.5" x14ac:dyDescent="0.45">
@@ -2815,14 +2827,14 @@
     </row>
     <row r="5" spans="2:7" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B5" s="100" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D5" s="101"/>
       <c r="F5" s="100" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G5" s="102" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="22.5" x14ac:dyDescent="0.45">
@@ -2830,25 +2842,21 @@
         <v>147</v>
       </c>
       <c r="D6" s="101" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E6" s="101" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F6" s="101"/>
     </row>
     <row r="7" spans="2:7" ht="22.5" x14ac:dyDescent="0.45">
-      <c r="B7" s="103" t="s">
-        <v>148</v>
-      </c>
+      <c r="B7" s="103"/>
       <c r="D7" s="101"/>
       <c r="E7" s="101"/>
       <c r="F7" s="101"/>
     </row>
     <row r="8" spans="2:7" ht="22.5" x14ac:dyDescent="0.45">
-      <c r="B8" s="103" t="s">
-        <v>149</v>
-      </c>
+      <c r="B8" s="103"/>
       <c r="D8" s="101"/>
       <c r="E8" s="101"/>
       <c r="F8" s="101"/>
@@ -2887,7 +2895,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="22.5" x14ac:dyDescent="0.45">
       <c r="A1" s="67" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="20"/>
@@ -2903,7 +2911,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" s="21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="58" t="str">
@@ -2920,7 +2928,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" s="21" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="59"/>
@@ -2929,7 +2937,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" s="66" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B6" s="66"/>
       <c r="C6" s="58" t="str">
@@ -2941,7 +2949,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" s="66" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B7" s="66"/>
       <c r="C7" s="58">
@@ -2953,7 +2961,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="66" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B8" s="66"/>
       <c r="C8" s="58">
@@ -2967,10 +2975,10 @@
     <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="D11" s="79"/>
       <c r="E11" s="60" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F11" s="60" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G11" s="61"/>
     </row>
@@ -2988,29 +2996,29 @@
     </row>
     <row r="13" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D13" s="62" t="s">
+        <v>157</v>
+      </c>
+      <c r="E13" s="81" t="s">
+        <v>158</v>
+      </c>
+      <c r="F13" s="85" t="s">
         <v>159</v>
-      </c>
-      <c r="E13" s="81" t="s">
-        <v>160</v>
-      </c>
-      <c r="F13" s="85" t="s">
-        <v>161</v>
       </c>
       <c r="G13" s="63"/>
       <c r="I13" s="78"/>
     </row>
     <row r="16" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C16" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="D16" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>164</v>
-      </c>
       <c r="F16" s="73" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H16" s="73"/>
       <c r="I16" s="73"/>
@@ -3028,10 +3036,10 @@
         <v>88</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F17" s="93">
         <v>0.75</v>
@@ -3050,10 +3058,10 @@
     <row r="18" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C18" s="21"/>
       <c r="D18" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F18" s="93">
         <v>1.25</v>
@@ -3071,13 +3079,13 @@
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C19" s="21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F19" s="93">
         <v>1</v>
@@ -3096,10 +3104,10 @@
     <row r="20" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C20" s="21"/>
       <c r="D20" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E20" s="17" t="s">
         <v>169</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>171</v>
       </c>
       <c r="F20" s="93">
         <v>2</v>
@@ -3117,10 +3125,10 @@
     </row>
     <row r="21" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C21" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>170</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>172</v>
       </c>
       <c r="E21" s="64">
         <v>50</v>
@@ -3129,7 +3137,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H21" s="72"/>
       <c r="I21" s="72"/>
@@ -3144,7 +3152,7 @@
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.45">
       <c r="D22" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E22" s="64">
         <v>150</v>
@@ -3153,7 +3161,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H22" s="72"/>
       <c r="I22" s="72"/>
@@ -3195,11 +3203,11 @@
     <row r="25" spans="3:17" x14ac:dyDescent="0.45">
       <c r="E25" s="74"/>
       <c r="G25" s="73" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H25" s="72"/>
       <c r="I25" s="86" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J25" s="72"/>
       <c r="K25" s="72"/>
@@ -3212,22 +3220,22 @@
     </row>
     <row r="26" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C26" s="21" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F26" s="73" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J26" s="73" t="s">
         <v>52</v>
@@ -3239,13 +3247,13 @@
         <v>75</v>
       </c>
       <c r="M26" s="75" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N26" s="31"/>
     </row>
     <row r="27" spans="3:17" x14ac:dyDescent="0.45">
       <c r="D27" s="17" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E27" s="64">
         <v>50</v>
@@ -3301,13 +3309,13 @@
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C30" s="21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>76</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F30" s="93">
         <v>1</v>
@@ -3323,10 +3331,10 @@
     </row>
     <row r="31" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C31" s="92" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F31" s="93">
         <v>1</v>
@@ -3360,9 +3368,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3382,7 +3390,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="22.9" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="110" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B1" s="111"/>
       <c r="H1" s="116"/>
@@ -3390,7 +3398,7 @@
     </row>
     <row r="2" spans="1:10" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="119" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B2" s="111"/>
       <c r="C2" s="120" t="str">
@@ -3407,28 +3415,28 @@
       <c r="C3" s="120"/>
       <c r="H3" s="122">
         <f>SUM(G12:G120)</f>
-        <v>0.14027777777777783</v>
+        <v>0.44791666666666641</v>
       </c>
       <c r="I3" s="118" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="119" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C4" s="124"/>
       <c r="H4" s="125">
         <f>(INT(H3*24))+MINUTE(H3)/60</f>
-        <v>3.3666666666666667</v>
+        <v>10.75</v>
       </c>
       <c r="I4" s="118" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="126" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B5" s="111"/>
       <c r="C5" s="120" t="str">
@@ -3439,7 +3447,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="126" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B6" s="127"/>
       <c r="C6" s="120">
@@ -3450,7 +3458,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="126" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B7" s="127"/>
       <c r="C7" s="120">
@@ -3467,19 +3475,19 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C9" s="128" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D9" s="129" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I9" s="117"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C10" s="128" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D10" s="129" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I10" s="126"/>
     </row>
@@ -3494,7 +3502,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="132" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G11" s="133" t="s">
         <v>3</v>
@@ -3522,6 +3530,9 @@
       <c r="G12" s="115">
         <f>(E12-D12)-(F12/1440)</f>
         <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="I12" s="118" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
@@ -3539,6 +3550,9 @@
         <f t="shared" ref="G13:G76" si="0">(E13-D13)-(F13/1440)</f>
         <v>4.861111111111116E-2</v>
       </c>
+      <c r="I13" s="118" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C14" s="112">
@@ -3554,110 +3568,206 @@
         <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
+      <c r="I14" s="118" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C15" s="112">
+        <v>43016</v>
+      </c>
+      <c r="D15" s="113">
+        <v>0.68472222222222223</v>
+      </c>
+      <c r="E15" s="113">
+        <v>0.70972222222222225</v>
+      </c>
       <c r="G15" s="115">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5000000000000022E-2</v>
+      </c>
+      <c r="I15" s="118" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C16" s="112">
+        <v>43016</v>
+      </c>
+      <c r="D16" s="113">
+        <v>0.70972222222222225</v>
+      </c>
+      <c r="E16" s="113">
+        <v>0.74583333333333324</v>
+      </c>
       <c r="G16" s="115">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.45">
+        <v>3.6111111111110983E-2</v>
+      </c>
+      <c r="H16" s="118" t="s">
+        <v>284</v>
+      </c>
+      <c r="I16" s="118" t="s">
+        <v>52</v>
+      </c>
+      <c r="J16" s="118" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="C17" s="112">
+        <v>43016</v>
+      </c>
+      <c r="D17" s="113">
+        <v>0.82500000000000007</v>
+      </c>
+      <c r="E17" s="113">
+        <v>0.91180555555555554</v>
+      </c>
       <c r="G17" s="115">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.45">
+        <v>8.6805555555555469E-2</v>
+      </c>
+      <c r="H17" s="118" t="s">
+        <v>284</v>
+      </c>
+      <c r="I17" s="118" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="C18" s="112">
+        <v>43017</v>
+      </c>
+      <c r="D18" s="113">
+        <v>0.50069444444444444</v>
+      </c>
+      <c r="E18" s="113">
+        <v>0.60486111111111118</v>
+      </c>
       <c r="G18" s="115">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.45">
+        <v>0.10416666666666674</v>
+      </c>
+      <c r="H18" s="118" t="s">
+        <v>286</v>
+      </c>
+      <c r="I18" s="118" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="C19" s="112">
+        <v>43017</v>
+      </c>
+      <c r="D19" s="113">
+        <v>0.60486111111111118</v>
+      </c>
+      <c r="E19" s="113">
+        <v>0.61458333333333337</v>
+      </c>
       <c r="G19" s="115">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.45">
+        <v>9.7222222222221877E-3</v>
+      </c>
+      <c r="H19" s="118" t="s">
+        <v>287</v>
+      </c>
+      <c r="I19" s="118" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="C20" s="112">
+        <v>43017</v>
+      </c>
+      <c r="D20" s="113">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="E20" s="113">
+        <v>0.74583333333333324</v>
+      </c>
       <c r="G20" s="115">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.45">
+        <v>4.5833333333333171E-2</v>
+      </c>
+      <c r="H20" s="118" t="s">
+        <v>288</v>
+      </c>
+      <c r="I20" s="118" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20" s="118" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.45">
       <c r="G21" s="115">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.45">
       <c r="G22" s="115">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.45">
       <c r="G23" s="115">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.45">
       <c r="G24" s="115">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.45">
       <c r="G25" s="115">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.45">
       <c r="G26" s="115">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.45">
       <c r="G27" s="115">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.45">
       <c r="G28" s="115">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.45">
       <c r="G29" s="115">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:10" x14ac:dyDescent="0.45">
       <c r="G30" s="115">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="3:10" x14ac:dyDescent="0.45">
       <c r="G31" s="115">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="3:10" x14ac:dyDescent="0.45">
       <c r="G32" s="115">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4241,13 +4351,13 @@
   <sheetData>
     <row r="1" spans="1:15" ht="22.9" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="65" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:15" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="54" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="55" t="str">
@@ -4266,12 +4376,12 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="54" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="87"/>
@@ -4281,12 +4391,12 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="68" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="55" t="str">
@@ -4297,7 +4407,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="68" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B6" s="66"/>
       <c r="C6" s="55">
@@ -4307,7 +4417,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="68" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B7" s="66"/>
       <c r="C7" s="55">
@@ -4320,18 +4430,18 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C9" s="88" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D9" s="89" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C10" s="88" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D10" s="89" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
@@ -4348,7 +4458,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="91" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>3</v>
@@ -4372,7 +4482,7 @@
         <v>56</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>7</v>
@@ -5114,7 +5224,7 @@
   <dimension ref="A1:F119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A26" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
@@ -5209,7 +5319,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>63</v>
@@ -5249,10 +5359,10 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C17" s="24" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.45">
@@ -5276,7 +5386,7 @@
         <v>52</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.45">
@@ -5284,7 +5394,7 @@
         <v>71</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.45">
@@ -5300,7 +5410,7 @@
         <v>74</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.45">
@@ -5308,7 +5418,7 @@
         <v>75</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.45">
@@ -5316,23 +5426,23 @@
         <v>76</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C26" s="24" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C27" s="24" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -5489,7 +5599,7 @@
         <v>137</v>
       </c>
       <c r="C53" s="96" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D53" s="17" t="s">
         <v>117</v>
@@ -5497,7 +5607,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C54" s="96" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D54" s="17" t="s">
         <v>118</v>
@@ -5505,7 +5615,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C55" s="96" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D55" s="17" t="s">
         <v>119</v>
@@ -5513,7 +5623,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C56" s="96" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D56" s="17" t="s">
         <v>120</v>
@@ -5521,7 +5631,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C57" s="96" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D57" s="17" t="s">
         <v>121</v>
@@ -5529,7 +5639,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C58" s="96" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D58" s="17" t="s">
         <v>122</v>
@@ -5537,7 +5647,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C59" s="96" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D59" s="17" t="s">
         <v>123</v>
@@ -5548,63 +5658,63 @@
         <v>138</v>
       </c>
       <c r="C60" s="42" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D60" s="31" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C61" s="42" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B62" s="31"/>
       <c r="C62" s="42" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D62" s="31" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B63" s="31"/>
       <c r="C63" s="42" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D63" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B64" s="31"/>
       <c r="C64" s="97" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D64" s="31" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B65" s="31"/>
       <c r="C65" s="42" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D65" s="31" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B66" s="31"/>
       <c r="C66" s="42" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D66" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.45">
@@ -5612,63 +5722,63 @@
         <v>129</v>
       </c>
       <c r="C67" s="95" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D67" s="31" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B68" s="31"/>
       <c r="C68" s="95" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B69" s="31"/>
       <c r="C69" s="95" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D69" s="31" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B70" s="31"/>
       <c r="C70" s="95" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D70" s="31" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C71" s="43" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D71" s="31" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B72" s="31"/>
       <c r="C72" s="43" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D72" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B73" s="31"/>
       <c r="C73" s="43" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D73" s="31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.45">
@@ -5676,40 +5786,40 @@
         <v>139</v>
       </c>
       <c r="C74" s="44" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D74" s="28"/>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C75" s="44" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D75" s="28"/>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C76" s="44" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D76" s="28"/>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C77" s="44" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D77" s="28"/>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C78" s="44" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D78" s="28"/>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C79" s="44" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D79" s="31" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.45">
@@ -5717,25 +5827,25 @@
         <v>140</v>
       </c>
       <c r="C80" s="45" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D80" s="28"/>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C81" s="45" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D81" s="28"/>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C82" s="45" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D82" s="28"/>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C83" s="45" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D83" s="31" t="s">
         <v>127</v>
@@ -5743,7 +5853,7 @@
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C84" s="45" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D84" s="31" t="s">
         <v>128</v>
@@ -5751,28 +5861,28 @@
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C85" s="45" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D85" s="28"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C86" s="45" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D86" s="28"/>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C87" s="45" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D87" s="28"/>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C88" s="45" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D88" s="31" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.45">
@@ -5780,25 +5890,25 @@
         <v>141</v>
       </c>
       <c r="C89" s="46" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D89" s="28"/>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C90" s="46" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D90" s="28"/>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C91" s="46" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D91" s="28"/>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C92" s="46" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D92" s="31" t="s">
         <v>132</v>
@@ -5806,7 +5916,7 @@
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C93" s="46" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D93" s="28"/>
     </row>
@@ -5815,37 +5925,37 @@
         <v>142</v>
       </c>
       <c r="C94" s="48" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D94" s="28"/>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C95" s="48" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D95" s="28"/>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C96" s="48" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D96" s="28"/>
     </row>
     <row r="97" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C97" s="48" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D97" s="28"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C98" s="48" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D98" s="28"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C99" s="48" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D99" s="28"/>
     </row>
@@ -5893,7 +6003,7 @@
       </c>
       <c r="C105" s="52"/>
       <c r="D105" s="17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -6102,7 +6212,7 @@
       <c r="P10" s="105"/>
     </row>
     <row r="11" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C11" s="109" t="s">
+      <c r="C11" s="106" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="105"/>
@@ -6157,7 +6267,7 @@
       <c r="O14" s="105"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="C15" s="106" t="s">
+      <c r="C15" s="107" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="105"/>
@@ -6199,7 +6309,7 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B18" s="13"/>
-      <c r="C18" s="108" t="s">
+      <c r="C18" s="109" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="105"/>
@@ -6218,7 +6328,7 @@
     <row r="19" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
-      <c r="D19" s="107" t="s">
+      <c r="D19" s="108" t="s">
         <v>32</v>
       </c>
       <c r="E19" s="105"/>
@@ -6235,7 +6345,7 @@
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B20" s="13"/>
-      <c r="C20" s="107" t="s">
+      <c r="C20" s="108" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="105"/>
@@ -6349,7 +6459,7 @@
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B26" s="13"/>
-      <c r="C26" s="107" t="s">
+      <c r="C26" s="108" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="105"/>
@@ -6410,7 +6520,7 @@
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="C32" s="106" t="s">
+      <c r="C32" s="107" t="s">
         <v>21</v>
       </c>
       <c r="D32" s="105"/>
@@ -6442,7 +6552,7 @@
       <c r="N34" s="105"/>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="C35" s="106" t="s">
+      <c r="C35" s="107" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="105"/>
@@ -6474,7 +6584,7 @@
       <c r="N37" s="105"/>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="C38" s="106" t="s">
+      <c r="C38" s="107" t="s">
         <v>25</v>
       </c>
       <c r="D38" s="105"/>
@@ -6491,12 +6601,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="D25:Q25"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="B6:P6"/>
-    <mergeCell ref="B7:P7"/>
-    <mergeCell ref="B10:P10"/>
-    <mergeCell ref="B12:P12"/>
     <mergeCell ref="C34:N34"/>
     <mergeCell ref="C35:N35"/>
     <mergeCell ref="C37:N37"/>
@@ -6513,6 +6617,12 @@
     <mergeCell ref="D22:N22"/>
     <mergeCell ref="D23:Q23"/>
     <mergeCell ref="D24:Q24"/>
+    <mergeCell ref="D25:Q25"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="B6:P6"/>
+    <mergeCell ref="B7:P7"/>
+    <mergeCell ref="B10:P10"/>
+    <mergeCell ref="B12:P12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D8" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
@@ -6597,7 +6707,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.45">
@@ -6608,12 +6718,12 @@
         <v>13</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="D8" s="18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
@@ -6624,7 +6734,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="2:4" s="74" customFormat="1" x14ac:dyDescent="0.45">
@@ -6635,12 +6745,12 @@
         <v>13</v>
       </c>
       <c r="D10" s="74" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D11" s="17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
@@ -6651,12 +6761,12 @@
         <v>13</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D14" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="1000" spans="2:2" x14ac:dyDescent="0.45"/>

</xml_diff>